<commit_message>
Añadidos más datos al archivo de los censos
</commit_message>
<xml_diff>
--- a/censo.xlsx
+++ b/censo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="1820" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>nombre</t>
   </si>
@@ -48,13 +48,79 @@
   </si>
   <si>
     <t>fdshghg</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>75643234W</t>
+  </si>
+  <si>
+    <t>jkcfdasd</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Xurso</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>sergio@yomolomucho.es</t>
+  </si>
+  <si>
+    <t>david@gmail.com</t>
+  </si>
+  <si>
+    <t>santi@yomolomucho.es</t>
+  </si>
+  <si>
+    <t>xurso@gmail.com</t>
+  </si>
+  <si>
+    <t>adrian@yomolomucho.es</t>
+  </si>
+  <si>
+    <t>luis@gmail.com</t>
+  </si>
+  <si>
+    <t>12321543P</t>
+  </si>
+  <si>
+    <t>89098456D</t>
+  </si>
+  <si>
+    <t>12047623S</t>
+  </si>
+  <si>
+    <t>71234432X</t>
+  </si>
+  <si>
+    <t>56412376R</t>
+  </si>
+  <si>
+    <t>54234981Q</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,6 +132,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,16 +162,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,10 +487,116 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>